<commit_message>
PyPoll steps 1-6 complete!
</commit_message>
<xml_diff>
--- a/PyBank/Resources/Test Formulas.xlsx
+++ b/PyBank/Resources/Test Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\regin\Desktop\03-Python\Homework\Instructions\PyBank\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E7D657-D1A0-4DCC-9728-A480DA502595}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406F7F19-ABFC-4895-8771-2FE1F9A71508}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="675" windowWidth="18390" windowHeight="10365" xr2:uid="{663382B0-073A-4CA3-80CB-3B655B3CD017}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>greatest increase:</t>
+  </si>
+  <si>
+    <t>greatest decrease:</t>
   </si>
 </sst>
 </file>
@@ -436,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3423D0E3-D6BD-472A-84CE-F9322C8C4CA3}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,6 +448,7 @@
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -545,6 +549,13 @@
       <c r="H5" s="2">
         <f>B6-budget_data[[#This Row],[Profit/Losses]]</f>
         <v>379920</v>
+      </c>
+      <c r="K5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="2">
+        <f>MIN(H3:H86)</f>
+        <v>-2196167</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>